<commit_message>
Update on density and core plots.
</commit_message>
<xml_diff>
--- a/DepthDensity_Bcores_lowResAve.xlsx
+++ b/DepthDensity_Bcores_lowResAve.xlsx
@@ -3556,7 +3556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E189"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3596,3192 +3596,1070 @@
         <v>18.04</v>
       </c>
       <c r="B2" t="n">
-        <v>580.645161290324</v>
+        <v>569.8924731182792</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>15.2065974448747</v>
       </c>
       <c r="D2" t="n">
-        <v>8.18</v>
+        <v>8.175000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>18.35</v>
+        <v>18.965</v>
       </c>
       <c r="B3" t="n">
-        <v>548.3870967741893</v>
+        <v>571.6845878136215</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>21.36753915525381</v>
       </c>
       <c r="D3" t="n">
-        <v>8.35</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>18.66</v>
+        <v>19.87</v>
       </c>
       <c r="B4" t="n">
-        <v>580.645161290324</v>
+        <v>577.7777777777782</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>15.71348402636578</v>
       </c>
       <c r="D4" t="n">
-        <v>8.529999999999999</v>
+        <v>9.225000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>18.96</v>
+        <v>20.77</v>
       </c>
       <c r="B5" t="n">
-        <v>566.6666666666652</v>
+        <v>584.2911877394629</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>13.67553126250923</v>
       </c>
       <c r="D5" t="n">
-        <v>8.699999999999999</v>
+        <v>9.745000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>19.27</v>
+        <v>21.655</v>
       </c>
       <c r="B6" t="n">
-        <v>548.3870967741956</v>
+        <v>590.8045977011496</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>6.50213132125379</v>
       </c>
       <c r="D6" t="n">
-        <v>8.869999999999999</v>
+        <v>10.265</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>19.57</v>
+        <v>22.53</v>
       </c>
       <c r="B7" t="n">
-        <v>600.0000000000035</v>
+        <v>609.1954022988511</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>16.25532830313403</v>
       </c>
       <c r="D7" t="n">
-        <v>9.050000000000001</v>
+        <v>10.785</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>19.87</v>
+        <v>23.4</v>
       </c>
       <c r="B8" t="n">
-        <v>566.6666666666652</v>
+        <v>605.0903119868636</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>26.70518221230293</v>
       </c>
       <c r="D8" t="n">
-        <v>9.220000000000001</v>
+        <v>11.31</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>20.17</v>
+        <v>24.255</v>
       </c>
       <c r="B9" t="n">
-        <v>599.9999999999976</v>
+        <v>612.0689655172401</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>23.38820941419822</v>
       </c>
       <c r="D9" t="n">
-        <v>9.4</v>
+        <v>11.835</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>20.47</v>
+        <v>25.105</v>
       </c>
       <c r="B10" t="n">
-        <v>566.6666666666717</v>
+        <v>612.0689655172398</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>23.388209414192</v>
       </c>
       <c r="D10" t="n">
-        <v>9.57</v>
+        <v>12.355</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>20.77</v>
+        <v>25.95</v>
       </c>
       <c r="B11" t="n">
-        <v>566.6666666666652</v>
+        <v>626.5432098765463</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>14.74272795176937</v>
       </c>
       <c r="D11" t="n">
-        <v>9.74</v>
+        <v>12.875</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>21.07</v>
+        <v>26.78</v>
       </c>
       <c r="B12" t="n">
-        <v>599.9999999999976</v>
+        <v>638.8888888888893</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>24.46196032923962</v>
       </c>
       <c r="D12" t="n">
-        <v>9.92</v>
+        <v>13.395</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>21.36</v>
+        <v>27.605</v>
       </c>
       <c r="B13" t="n">
-        <v>586.2068965517257</v>
+        <v>634.4797178130502</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>24.5413052029541</v>
       </c>
       <c r="D13" t="n">
-        <v>10.09</v>
+        <v>13.92</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>21.66</v>
+        <v>28.43</v>
       </c>
       <c r="B14" t="n">
-        <v>599.9999999999976</v>
+        <v>631.0588092197303</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>9.106089291928123</v>
       </c>
       <c r="D14" t="n">
-        <v>10.27</v>
+        <v>14.445</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>21.95</v>
+        <v>29.27</v>
       </c>
       <c r="B15" t="n">
-        <v>586.2068965517257</v>
+        <v>654.7619047619035</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>16.83587574253451</v>
       </c>
       <c r="D15" t="n">
-        <v>10.44</v>
+        <v>14.985</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>22.24</v>
+        <v>30.11</v>
       </c>
       <c r="B16" t="n">
-        <v>586.2068965517257</v>
+        <v>654.7619047619029</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>16.83587574253493</v>
       </c>
       <c r="D16" t="n">
-        <v>10.61</v>
+        <v>15.53</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>22.53</v>
+        <v>30.95</v>
       </c>
       <c r="B17" t="n">
-        <v>620.689655172407</v>
+        <v>650.7936507936532</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>11.22391716168952</v>
       </c>
       <c r="D17" t="n">
-        <v>10.79</v>
+        <v>16.08</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>22.82</v>
+        <v>31.775</v>
       </c>
       <c r="B18" t="n">
-        <v>586.2068965517318</v>
+        <v>663.1393298059946</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>28.68334385765797</v>
       </c>
       <c r="D18" t="n">
-        <v>10.96</v>
+        <v>16.625</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>23.11</v>
+        <v>32.59999999999999</v>
       </c>
       <c r="B19" t="n">
-        <v>620.6896551724146</v>
+        <v>658.7301587301619</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>11.22391716169603</v>
       </c>
       <c r="D19" t="n">
-        <v>11.14</v>
+        <v>17.17</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>23.4</v>
+        <v>33.42</v>
       </c>
       <c r="B20" t="n">
-        <v>586.2068965517257</v>
+        <v>679.0123456790068</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>17.45942669595636</v>
       </c>
       <c r="D20" t="n">
-        <v>11.31</v>
+        <v>17.715</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>23.69</v>
+        <v>34.23</v>
       </c>
       <c r="B21" t="n">
-        <v>586.2068965517184</v>
+        <v>679.0123456790112</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>17.45942669595325</v>
       </c>
       <c r="D21" t="n">
-        <v>11.48</v>
+        <v>18.26</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>23.97</v>
+        <v>35.035</v>
       </c>
       <c r="B22" t="n">
-        <v>642.8571428571473</v>
+        <v>675.213675213681</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>12.08729540489713</v>
       </c>
       <c r="D22" t="n">
-        <v>11.66</v>
+        <v>18.81</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>24.26</v>
+        <v>35.835</v>
       </c>
       <c r="B23" t="n">
-        <v>586.2068965517184</v>
+        <v>687.5593542260198</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>15.48861009524251</v>
       </c>
       <c r="D23" t="n">
-        <v>11.83</v>
+        <v>19.355</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>24.54</v>
+        <v>36.63</v>
       </c>
       <c r="B24" t="n">
-        <v>642.8571428571473</v>
+        <v>683.7606837606876</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>12.08729540488544</v>
       </c>
       <c r="D24" t="n">
-        <v>12.01</v>
+        <v>19.9</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24.82</v>
+        <v>37.42</v>
       </c>
       <c r="B25" t="n">
-        <v>607.1428571428544</v>
+        <v>696.5811965811876</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>26.34364958534027</v>
       </c>
       <c r="D25" t="n">
-        <v>12.18</v>
+        <v>20.445</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25.11</v>
+        <v>38.21</v>
       </c>
       <c r="B26" t="n">
-        <v>586.2068965517257</v>
+        <v>692.307692307701</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>6.437379080603477e-12</v>
       </c>
       <c r="D26" t="n">
-        <v>12.35</v>
+        <v>20.99</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>25.39</v>
+        <v>38.98999999999999</v>
       </c>
       <c r="B27" t="n">
-        <v>642.8571428571393</v>
+        <v>705.1282051282003</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>18.13094310733448</v>
       </c>
       <c r="D27" t="n">
-        <v>12.53</v>
+        <v>21.535</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>25.67</v>
+        <v>39.765</v>
       </c>
       <c r="B28" t="n">
-        <v>607.1428571428544</v>
+        <v>714.3589743589728</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>16.20058358865461</v>
       </c>
       <c r="D28" t="n">
-        <v>12.7</v>
+        <v>22.08</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>25.95</v>
+        <v>40.54</v>
       </c>
       <c r="B29" t="n">
-        <v>642.8571428571538</v>
+        <v>701.538461538464</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>13.05427903728759</v>
       </c>
       <c r="D29" t="n">
-        <v>12.88</v>
+        <v>22.63</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>26.23</v>
+        <v>41.305</v>
       </c>
       <c r="B30" t="n">
-        <v>607.1428571428544</v>
+        <v>714.8717948717929</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>31.91045986892633</v>
       </c>
       <c r="D30" t="n">
-        <v>13.05</v>
+        <v>23.175</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>26.5</v>
+        <v>42.075</v>
       </c>
       <c r="B31" t="n">
-        <v>629.6296296296304</v>
+        <v>710.7692307692314</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>13.05427903728759</v>
       </c>
       <c r="D31" t="n">
-        <v>13.22</v>
+        <v>23.72</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>26.78</v>
+        <v>42.835</v>
       </c>
       <c r="B32" t="n">
-        <v>642.8571428571393</v>
+        <v>723.5897435897396</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>5.076664070053332</v>
       </c>
       <c r="D32" t="n">
-        <v>13.4</v>
+        <v>24.265</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>27.06</v>
+        <v>43.595</v>
       </c>
       <c r="B33" t="n">
-        <v>607.1428571428621</v>
+        <v>724.1025641025668</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>27.78711217260387</v>
       </c>
       <c r="D33" t="n">
-        <v>13.57</v>
+        <v>24.81</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>27.33</v>
+        <v>44.35</v>
       </c>
       <c r="B34" t="n">
-        <v>666.6666666666666</v>
+        <v>719.9999999999989</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>13.75</v>
+        <v>25.36</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>27.6</v>
+        <v>45.1</v>
       </c>
       <c r="B35" t="n">
-        <v>629.6296296296221</v>
+        <v>733.3333333333343</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>18.85618083164421</v>
       </c>
       <c r="D35" t="n">
-        <v>13.92</v>
+        <v>25.905</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>27.88</v>
+        <v>45.85</v>
       </c>
       <c r="B36" t="n">
-        <v>607.1428571428621</v>
+        <v>729.9999999999968</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>14.14213562372798</v>
       </c>
       <c r="D36" t="n">
-        <v>14.09</v>
+        <v>26.45</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>28.15</v>
+        <v>46.59</v>
       </c>
       <c r="B37" t="n">
-        <v>666.6666666666666</v>
+        <v>733.3333333333343</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>18.85618083164421</v>
       </c>
       <c r="D37" t="n">
-        <v>14.27</v>
+        <v>26.995</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>28.42</v>
+        <v>47.335</v>
       </c>
       <c r="B38" t="n">
-        <v>629.6296296296221</v>
+        <v>730.0000000000041</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>14.14213562373845</v>
       </c>
       <c r="D38" t="n">
-        <v>14.44</v>
+        <v>27.54</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>28.71</v>
+        <v>48.075</v>
       </c>
       <c r="B39" t="n">
-        <v>620.6896551724146</v>
+        <v>753.8888888888856</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>29.38673590097399</v>
       </c>
       <c r="D39" t="n">
-        <v>14.62</v>
+        <v>28.085</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>28.99</v>
+        <v>48.805</v>
       </c>
       <c r="B40" t="n">
-        <v>642.8571428571538</v>
+        <v>743.3333333333395</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>16.99673171198007</v>
       </c>
       <c r="D40" t="n">
-        <v>14.8</v>
+        <v>28.63</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>29.27</v>
+        <v>49.54</v>
       </c>
       <c r="B41" t="n">
-        <v>678.571428571424</v>
+        <v>739.9999999999945</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>14.14213562372798</v>
       </c>
       <c r="D41" t="n">
-        <v>14.99</v>
+        <v>29.18</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>29.55</v>
+        <v>50.27</v>
       </c>
       <c r="B42" t="n">
-        <v>642.8571428571393</v>
+        <v>753.8888888888933</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>29.38673590098403</v>
       </c>
       <c r="D42" t="n">
-        <v>15.17</v>
+        <v>29.725</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>29.83</v>
+        <v>51</v>
       </c>
       <c r="B43" t="n">
-        <v>642.8571428571473</v>
+        <v>750</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>1.046734847820651e-11</v>
       </c>
       <c r="D43" t="n">
-        <v>15.35</v>
+        <v>30.27</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>30.11</v>
+        <v>51.72</v>
       </c>
       <c r="B44" t="n">
-        <v>642.8571428571393</v>
+        <v>763.8888888888835</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>19.64185503296257</v>
       </c>
       <c r="D44" t="n">
-        <v>15.53</v>
+        <v>30.815</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>30.39</v>
+        <v>52.44</v>
       </c>
       <c r="B45" t="n">
-        <v>642.8571428571456</v>
+        <v>763.888888888891</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>19.64185503295733</v>
       </c>
       <c r="D45" t="n">
-        <v>15.71</v>
+        <v>31.36</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>30.67</v>
+        <v>53.165</v>
       </c>
       <c r="B46" t="n">
-        <v>678.571428571424</v>
+        <v>753.8888888888927</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>29.38673590096122</v>
       </c>
       <c r="D46" t="n">
-        <v>15.9</v>
+        <v>31.91</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>30.95</v>
+        <v>53.895</v>
       </c>
       <c r="B47" t="n">
-        <v>642.8571428571411</v>
+        <v>756.6666666666677</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>4.714045207916235</v>
       </c>
       <c r="D47" t="n">
-        <v>16.08</v>
+        <v>32.465</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>31.23</v>
+        <v>54.63500000000001</v>
       </c>
       <c r="B48" t="n">
-        <v>642.8571428571519</v>
+        <v>767.2222222222186</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>17.7604081812622</v>
       </c>
       <c r="D48" t="n">
-        <v>16.26</v>
+        <v>33.03</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>31.5</v>
+        <v>55.36499999999999</v>
       </c>
       <c r="B49" t="n">
-        <v>666.6666666666666</v>
+        <v>767.2222222222213</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>17.76040818128297</v>
       </c>
       <c r="D49" t="n">
-        <v>16.44</v>
+        <v>33.59</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>31.78</v>
+        <v>56.09</v>
       </c>
       <c r="B50" t="n">
-        <v>642.8571428571393</v>
+        <v>767.7777777777844</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>33.78399065669609</v>
       </c>
       <c r="D50" t="n">
-        <v>16.62</v>
+        <v>34.15000000000001</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>32.05</v>
+        <v>56.82</v>
       </c>
       <c r="B51" t="n">
-        <v>703.7037037037056</v>
+        <v>777.777777777772</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>19.64185503294514</v>
       </c>
       <c r="D51" t="n">
-        <v>16.81</v>
+        <v>34.71</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>32.33</v>
+        <v>57.54</v>
       </c>
       <c r="B52" t="n">
-        <v>642.8571428571393</v>
+        <v>777.7777777777744</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>19.6418550329626</v>
       </c>
       <c r="D52" t="n">
-        <v>16.99</v>
+        <v>35.27</v>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>32.6</v>
+        <v>58.26000000000001</v>
       </c>
       <c r="B53" t="n">
-        <v>666.6666666666711</v>
+        <v>791.6666666666683</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1.276338064850716e-11</v>
       </c>
       <c r="D53" t="n">
-        <v>17.17</v>
+        <v>35.83</v>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>32.87</v>
+        <v>58.98</v>
       </c>
       <c r="B54" t="n">
-        <v>666.6666666666754</v>
+        <v>777.7777777777818</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>19.64185503295213</v>
       </c>
       <c r="D54" t="n">
-        <v>17.35</v>
+        <v>36.395</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>33.15</v>
+        <v>59.7</v>
       </c>
       <c r="B55" t="n">
-        <v>642.8571428571393</v>
+        <v>777.7777777777724</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>19.64185503296113</v>
       </c>
       <c r="D55" t="n">
-        <v>17.53</v>
+        <v>36.955</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>33.42</v>
+        <v>60.415</v>
       </c>
       <c r="B56" t="n">
-        <v>703.7037037036872</v>
+        <v>789.2512077294715</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>31.10929196231315</v>
       </c>
       <c r="D56" t="n">
-        <v>17.72</v>
+        <v>37.515</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>33.69</v>
+        <v>61.13</v>
       </c>
       <c r="B57" t="n">
-        <v>666.6666666666754</v>
+        <v>789.2512077294708</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>31.10929196230368</v>
       </c>
       <c r="D57" t="n">
-        <v>17.9</v>
+        <v>38.075</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>33.96</v>
+        <v>61.84</v>
       </c>
       <c r="B58" t="n">
-        <v>666.6666666666579</v>
+        <v>789.2512077294605</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>31.10929196229149</v>
       </c>
       <c r="D58" t="n">
-        <v>18.08</v>
+        <v>38.63500000000001</v>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>34.23</v>
+        <v>62.545</v>
       </c>
       <c r="B59" t="n">
-        <v>666.6666666666886</v>
+        <v>788.6473429951711</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>4.269968485437911</v>
       </c>
       <c r="D59" t="n">
-        <v>18.26</v>
+        <v>39.195</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>34.5</v>
+        <v>63.255</v>
       </c>
       <c r="B60" t="n">
-        <v>666.6666666666579</v>
+        <v>800.7246376811681</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>35.86773527758992</v>
       </c>
       <c r="D60" t="n">
-        <v>18.44</v>
+        <v>39.755</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>34.77</v>
+        <v>63.955</v>
       </c>
       <c r="B61" t="n">
-        <v>703.7037037036872</v>
+        <v>789.9494949494797</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>23.78364284917284</v>
       </c>
       <c r="D61" t="n">
-        <v>18.63</v>
+        <v>40.315</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>35.03</v>
+        <v>64.66500000000001</v>
       </c>
       <c r="B62" t="n">
-        <v>692.3076923076965</v>
+        <v>800.7246376811778</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>35.86773527761241</v>
       </c>
       <c r="D62" t="n">
-        <v>18.81</v>
+        <v>40.875</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>35.3</v>
+        <v>65.36499999999999</v>
       </c>
       <c r="B63" t="n">
-        <v>666.6666666666754</v>
+        <v>800.7246376811585</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>35.86773527756741</v>
       </c>
       <c r="D63" t="n">
-        <v>18.99</v>
+        <v>41.435</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>35.57</v>
+        <v>65.62344919786096</v>
       </c>
       <c r="B64" t="n">
-        <v>666.6666666666711</v>
+        <v>826.0869565217149</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>19.17</v>
+        <v>41.61681818181818</v>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>35.83</v>
-      </c>
-      <c r="B65" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C65" t="n">
-        <v>0</v>
-      </c>
-      <c r="D65" t="n">
-        <v>19.35</v>
-      </c>
-      <c r="E65" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>36.1</v>
-      </c>
-      <c r="B66" t="n">
-        <v>703.7037037036872</v>
-      </c>
-      <c r="C66" t="n">
-        <v>0</v>
-      </c>
-      <c r="D66" t="n">
-        <v>19.54</v>
-      </c>
-      <c r="E66" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>36.37</v>
-      </c>
-      <c r="B67" t="n">
-        <v>666.6666666666754</v>
-      </c>
-      <c r="C67" t="n">
-        <v>0</v>
-      </c>
-      <c r="D67" t="n">
-        <v>19.72</v>
-      </c>
-      <c r="E67" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>36.63</v>
-      </c>
-      <c r="B68" t="n">
-        <v>692.3076923076776</v>
-      </c>
-      <c r="C68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D68" t="n">
-        <v>19.9</v>
-      </c>
-      <c r="E68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>36.89</v>
-      </c>
-      <c r="B69" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C69" t="n">
-        <v>0</v>
-      </c>
-      <c r="D69" t="n">
-        <v>20.08</v>
-      </c>
-      <c r="E69" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>37.16</v>
-      </c>
-      <c r="B70" t="n">
-        <v>666.6666666666886</v>
-      </c>
-      <c r="C70" t="n">
-        <v>0</v>
-      </c>
-      <c r="D70" t="n">
-        <v>20.26</v>
-      </c>
-      <c r="E70" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>37.42</v>
-      </c>
-      <c r="B71" t="n">
-        <v>692.3076923076776</v>
-      </c>
-      <c r="C71" t="n">
-        <v>0</v>
-      </c>
-      <c r="D71" t="n">
-        <v>20.44</v>
-      </c>
-      <c r="E71" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>37.68</v>
-      </c>
-      <c r="B72" t="n">
-        <v>730.7692307692276</v>
-      </c>
-      <c r="C72" t="n">
-        <v>0</v>
-      </c>
-      <c r="D72" t="n">
-        <v>20.63</v>
-      </c>
-      <c r="E72" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>37.95</v>
-      </c>
-      <c r="B73" t="n">
-        <v>666.6666666666579</v>
-      </c>
-      <c r="C73" t="n">
-        <v>0</v>
-      </c>
-      <c r="D73" t="n">
-        <v>20.81</v>
-      </c>
-      <c r="E73" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>38.21</v>
-      </c>
-      <c r="B74" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C74" t="n">
-        <v>0</v>
-      </c>
-      <c r="D74" t="n">
-        <v>20.99</v>
-      </c>
-      <c r="E74" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>38.47</v>
-      </c>
-      <c r="B75" t="n">
-        <v>692.3076923077101</v>
-      </c>
-      <c r="C75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D75" t="n">
-        <v>21.17</v>
-      </c>
-      <c r="E75" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>38.73</v>
-      </c>
-      <c r="B76" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C76" t="n">
-        <v>0</v>
-      </c>
-      <c r="D76" t="n">
-        <v>21.35</v>
-      </c>
-      <c r="E76" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>38.99</v>
-      </c>
-      <c r="B77" t="n">
-        <v>730.7692307692076</v>
-      </c>
-      <c r="C77" t="n">
-        <v>0</v>
-      </c>
-      <c r="D77" t="n">
-        <v>21.54</v>
-      </c>
-      <c r="E77" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>39.25</v>
-      </c>
-      <c r="B78" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C78" t="n">
-        <v>0</v>
-      </c>
-      <c r="D78" t="n">
-        <v>21.72</v>
-      </c>
-      <c r="E78" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>39.51</v>
-      </c>
-      <c r="B79" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C79" t="n">
-        <v>0</v>
-      </c>
-      <c r="D79" t="n">
-        <v>21.9</v>
-      </c>
-      <c r="E79" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>39.77</v>
-      </c>
-      <c r="B80" t="n">
-        <v>692.3076923076776</v>
-      </c>
-      <c r="C80" t="n">
-        <v>0</v>
-      </c>
-      <c r="D80" t="n">
-        <v>22.08</v>
-      </c>
-      <c r="E80" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>40.02</v>
-      </c>
-      <c r="B81" t="n">
-        <v>720.0000000000131</v>
-      </c>
-      <c r="C81" t="n">
-        <v>0</v>
-      </c>
-      <c r="D81" t="n">
-        <v>22.26</v>
-      </c>
-      <c r="E81" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>40.28</v>
-      </c>
-      <c r="B82" t="n">
-        <v>730.7692307692276</v>
-      </c>
-      <c r="C82" t="n">
-        <v>0</v>
-      </c>
-      <c r="D82" t="n">
-        <v>22.45</v>
-      </c>
-      <c r="E82" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>40.54</v>
-      </c>
-      <c r="B83" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D83" t="n">
-        <v>22.63</v>
-      </c>
-      <c r="E83" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>40.8</v>
-      </c>
-      <c r="B84" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C84" t="n">
-        <v>0</v>
-      </c>
-      <c r="D84" t="n">
-        <v>22.81</v>
-      </c>
-      <c r="E84" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>41.05</v>
-      </c>
-      <c r="B85" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C85" t="n">
-        <v>0</v>
-      </c>
-      <c r="D85" t="n">
-        <v>22.99</v>
-      </c>
-      <c r="E85" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>41.31</v>
-      </c>
-      <c r="B86" t="n">
-        <v>692.3076923076912</v>
-      </c>
-      <c r="C86" t="n">
-        <v>0</v>
-      </c>
-      <c r="D86" t="n">
-        <v>23.17</v>
-      </c>
-      <c r="E86" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>41.56</v>
-      </c>
-      <c r="B87" t="n">
-        <v>759.9999999999909</v>
-      </c>
-      <c r="C87" t="n">
-        <v>0</v>
-      </c>
-      <c r="D87" t="n">
-        <v>23.36</v>
-      </c>
-      <c r="E87" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>41.82</v>
-      </c>
-      <c r="B88" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C88" t="n">
-        <v>0</v>
-      </c>
-      <c r="D88" t="n">
-        <v>23.54</v>
-      </c>
-      <c r="E88" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>42.07</v>
-      </c>
-      <c r="B89" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C89" t="n">
-        <v>0</v>
-      </c>
-      <c r="D89" t="n">
-        <v>23.72</v>
-      </c>
-      <c r="E89" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>42.33</v>
-      </c>
-      <c r="B90" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C90" t="n">
-        <v>0</v>
-      </c>
-      <c r="D90" t="n">
-        <v>23.9</v>
-      </c>
-      <c r="E90" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>42.58</v>
-      </c>
-      <c r="B91" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C91" t="n">
-        <v>0</v>
-      </c>
-      <c r="D91" t="n">
-        <v>24.08</v>
-      </c>
-      <c r="E91" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>42.84</v>
-      </c>
-      <c r="B92" t="n">
-        <v>730.7692307692213</v>
-      </c>
-      <c r="C92" t="n">
-        <v>0</v>
-      </c>
-      <c r="D92" t="n">
-        <v>24.27</v>
-      </c>
-      <c r="E92" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>43.09</v>
-      </c>
-      <c r="B93" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C93" t="n">
-        <v>0</v>
-      </c>
-      <c r="D93" t="n">
-        <v>24.45</v>
-      </c>
-      <c r="E93" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>43.34</v>
-      </c>
-      <c r="B94" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C94" t="n">
-        <v>0</v>
-      </c>
-      <c r="D94" t="n">
-        <v>24.63</v>
-      </c>
-      <c r="E94" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>43.59</v>
-      </c>
-      <c r="B95" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C95" t="n">
-        <v>0</v>
-      </c>
-      <c r="D95" t="n">
-        <v>24.81</v>
-      </c>
-      <c r="E95" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>43.85</v>
-      </c>
-      <c r="B96" t="n">
-        <v>692.3076923076965</v>
-      </c>
-      <c r="C96" t="n">
-        <v>0</v>
-      </c>
-      <c r="D96" t="n">
-        <v>24.99</v>
-      </c>
-      <c r="E96" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>44.1</v>
-      </c>
-      <c r="B97" t="n">
-        <v>760.0000000000051</v>
-      </c>
-      <c r="C97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D97" t="n">
-        <v>25.18</v>
-      </c>
-      <c r="E97" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>44.35</v>
-      </c>
-      <c r="B98" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C98" t="n">
-        <v>0</v>
-      </c>
-      <c r="D98" t="n">
-        <v>25.36</v>
-      </c>
-      <c r="E98" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>44.6</v>
-      </c>
-      <c r="B99" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C99" t="n">
-        <v>0</v>
-      </c>
-      <c r="D99" t="n">
-        <v>25.54</v>
-      </c>
-      <c r="E99" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>44.85</v>
-      </c>
-      <c r="B100" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C100" t="n">
-        <v>0</v>
-      </c>
-      <c r="D100" t="n">
-        <v>25.72</v>
-      </c>
-      <c r="E100" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>45.1</v>
-      </c>
-      <c r="B101" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C101" t="n">
-        <v>0</v>
-      </c>
-      <c r="D101" t="n">
-        <v>25.9</v>
-      </c>
-      <c r="E101" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>45.35</v>
-      </c>
-      <c r="B102" t="n">
-        <v>760.0000000000051</v>
-      </c>
-      <c r="C102" t="n">
-        <v>0</v>
-      </c>
-      <c r="D102" t="n">
-        <v>26.09</v>
-      </c>
-      <c r="E102" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>45.6</v>
-      </c>
-      <c r="B103" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C103" t="n">
-        <v>0</v>
-      </c>
-      <c r="D103" t="n">
-        <v>26.27</v>
-      </c>
-      <c r="E103" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>45.85</v>
-      </c>
-      <c r="B104" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C104" t="n">
-        <v>0</v>
-      </c>
-      <c r="D104" t="n">
-        <v>26.45</v>
-      </c>
-      <c r="E104" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>46.1</v>
-      </c>
-      <c r="B105" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D105" t="n">
-        <v>26.63</v>
-      </c>
-      <c r="E105" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>46.34</v>
-      </c>
-      <c r="B106" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C106" t="n">
-        <v>0</v>
-      </c>
-      <c r="D106" t="n">
-        <v>26.81</v>
-      </c>
-      <c r="E106" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>46.59</v>
-      </c>
-      <c r="B107" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C107" t="n">
-        <v>0</v>
-      </c>
-      <c r="D107" t="n">
-        <v>26.99</v>
-      </c>
-      <c r="E107" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>46.84</v>
-      </c>
-      <c r="B108" t="n">
-        <v>760.0000000000051</v>
-      </c>
-      <c r="C108" t="n">
-        <v>0</v>
-      </c>
-      <c r="D108" t="n">
-        <v>27.18</v>
-      </c>
-      <c r="E108" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>47.09</v>
-      </c>
-      <c r="B109" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C109" t="n">
-        <v>0</v>
-      </c>
-      <c r="D109" t="n">
-        <v>27.36</v>
-      </c>
-      <c r="E109" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>47.33</v>
-      </c>
-      <c r="B110" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C110" t="n">
-        <v>0</v>
-      </c>
-      <c r="D110" t="n">
-        <v>27.54</v>
-      </c>
-      <c r="E110" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>47.58</v>
-      </c>
-      <c r="B111" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C111" t="n">
-        <v>0</v>
-      </c>
-      <c r="D111" t="n">
-        <v>27.72</v>
-      </c>
-      <c r="E111" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>47.83</v>
-      </c>
-      <c r="B112" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C112" t="n">
-        <v>0</v>
-      </c>
-      <c r="D112" t="n">
-        <v>27.9</v>
-      </c>
-      <c r="E112" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>48.07</v>
-      </c>
-      <c r="B113" t="n">
-        <v>791.6666666666654</v>
-      </c>
-      <c r="C113" t="n">
-        <v>0</v>
-      </c>
-      <c r="D113" t="n">
-        <v>28.09</v>
-      </c>
-      <c r="E113" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>48.32</v>
-      </c>
-      <c r="B114" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C114" t="n">
-        <v>0</v>
-      </c>
-      <c r="D114" t="n">
-        <v>28.27</v>
-      </c>
-      <c r="E114" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n">
-        <v>48.56</v>
-      </c>
-      <c r="B115" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C115" t="n">
-        <v>0</v>
-      </c>
-      <c r="D115" t="n">
-        <v>28.45</v>
-      </c>
-      <c r="E115" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n">
-        <v>48.81</v>
-      </c>
-      <c r="B116" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C116" t="n">
-        <v>0</v>
-      </c>
-      <c r="D116" t="n">
-        <v>28.63</v>
-      </c>
-      <c r="E116" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="n">
-        <v>49.05</v>
-      </c>
-      <c r="B117" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C117" t="n">
-        <v>0</v>
-      </c>
-      <c r="D117" t="n">
-        <v>28.81</v>
-      </c>
-      <c r="E117" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="n">
-        <v>49.3</v>
-      </c>
-      <c r="B118" t="n">
-        <v>760.0000000000051</v>
-      </c>
-      <c r="C118" t="n">
-        <v>0</v>
-      </c>
-      <c r="D118" t="n">
-        <v>29</v>
-      </c>
-      <c r="E118" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>49.54</v>
-      </c>
-      <c r="B119" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C119" t="n">
-        <v>0</v>
-      </c>
-      <c r="D119" t="n">
-        <v>29.18</v>
-      </c>
-      <c r="E119" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n">
-        <v>49.78</v>
-      </c>
-      <c r="B120" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C120" t="n">
-        <v>0</v>
-      </c>
-      <c r="D120" t="n">
-        <v>29.36</v>
-      </c>
-      <c r="E120" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>50.03</v>
-      </c>
-      <c r="B121" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D121" t="n">
-        <v>29.54</v>
-      </c>
-      <c r="E121" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>50.27</v>
-      </c>
-      <c r="B122" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C122" t="n">
-        <v>0</v>
-      </c>
-      <c r="D122" t="n">
-        <v>29.72</v>
-      </c>
-      <c r="E122" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>50.51</v>
-      </c>
-      <c r="B123" t="n">
-        <v>791.6666666666888</v>
-      </c>
-      <c r="C123" t="n">
-        <v>0</v>
-      </c>
-      <c r="D123" t="n">
-        <v>29.91</v>
-      </c>
-      <c r="E123" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="n">
-        <v>50.76</v>
-      </c>
-      <c r="B124" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C124" t="n">
-        <v>0</v>
-      </c>
-      <c r="D124" t="n">
-        <v>30.09</v>
-      </c>
-      <c r="E124" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="n">
-        <v>51</v>
-      </c>
-      <c r="B125" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C125" t="n">
-        <v>0</v>
-      </c>
-      <c r="D125" t="n">
-        <v>30.27</v>
-      </c>
-      <c r="E125" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="n">
-        <v>51.24</v>
-      </c>
-      <c r="B126" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C126" t="n">
-        <v>0</v>
-      </c>
-      <c r="D126" t="n">
-        <v>30.45</v>
-      </c>
-      <c r="E126" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="n">
-        <v>51.48</v>
-      </c>
-      <c r="B127" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C127" t="n">
-        <v>0</v>
-      </c>
-      <c r="D127" t="n">
-        <v>30.63</v>
-      </c>
-      <c r="E127" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="n">
-        <v>51.72</v>
-      </c>
-      <c r="B128" t="n">
-        <v>791.6666666666654</v>
-      </c>
-      <c r="C128" t="n">
-        <v>0</v>
-      </c>
-      <c r="D128" t="n">
-        <v>30.82</v>
-      </c>
-      <c r="E128" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="n">
-        <v>51.96</v>
-      </c>
-      <c r="B129" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C129" t="n">
-        <v>0</v>
-      </c>
-      <c r="D129" t="n">
-        <v>31</v>
-      </c>
-      <c r="E129" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="n">
-        <v>52.2</v>
-      </c>
-      <c r="B130" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C130" t="n">
-        <v>0</v>
-      </c>
-      <c r="D130" t="n">
-        <v>31.18</v>
-      </c>
-      <c r="E130" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="n">
-        <v>52.44</v>
-      </c>
-      <c r="B131" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C131" t="n">
-        <v>0</v>
-      </c>
-      <c r="D131" t="n">
-        <v>31.36</v>
-      </c>
-      <c r="E131" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="n">
-        <v>52.68</v>
-      </c>
-      <c r="B132" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C132" t="n">
-        <v>0</v>
-      </c>
-      <c r="D132" t="n">
-        <v>31.54</v>
-      </c>
-      <c r="E132" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="n">
-        <v>52.92</v>
-      </c>
-      <c r="B133" t="n">
-        <v>791.6666666666654</v>
-      </c>
-      <c r="C133" t="n">
-        <v>0</v>
-      </c>
-      <c r="D133" t="n">
-        <v>31.73</v>
-      </c>
-      <c r="E133" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="n">
-        <v>53.16</v>
-      </c>
-      <c r="B134" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C134" t="n">
-        <v>0</v>
-      </c>
-      <c r="D134" t="n">
-        <v>31.91</v>
-      </c>
-      <c r="E134" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="n">
-        <v>53.41</v>
-      </c>
-      <c r="B135" t="n">
-        <v>720.0000000000131</v>
-      </c>
-      <c r="C135" t="n">
-        <v>0</v>
-      </c>
-      <c r="D135" t="n">
-        <v>32.09</v>
-      </c>
-      <c r="E135" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="n">
-        <v>53.65</v>
-      </c>
-      <c r="B136" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C136" t="n">
-        <v>0</v>
-      </c>
-      <c r="D136" t="n">
-        <v>32.28</v>
-      </c>
-      <c r="E136" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="n">
-        <v>53.9</v>
-      </c>
-      <c r="B137" t="n">
-        <v>759.9999999999909</v>
-      </c>
-      <c r="C137" t="n">
-        <v>0</v>
-      </c>
-      <c r="D137" t="n">
-        <v>32.47</v>
-      </c>
-      <c r="E137" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="n">
-        <v>54.14</v>
-      </c>
-      <c r="B138" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C138" t="n">
-        <v>0</v>
-      </c>
-      <c r="D138" t="n">
-        <v>32.65</v>
-      </c>
-      <c r="E138" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="n">
-        <v>54.39</v>
-      </c>
-      <c r="B139" t="n">
-        <v>760.0000000000193</v>
-      </c>
-      <c r="C139" t="n">
-        <v>0</v>
-      </c>
-      <c r="D139" t="n">
-        <v>32.84</v>
-      </c>
-      <c r="E139" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="n">
-        <v>54.63</v>
-      </c>
-      <c r="B140" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C140" t="n">
-        <v>0</v>
-      </c>
-      <c r="D140" t="n">
-        <v>33.03</v>
-      </c>
-      <c r="E140" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="n">
-        <v>54.88</v>
-      </c>
-      <c r="B141" t="n">
-        <v>759.9999999999909</v>
-      </c>
-      <c r="C141" t="n">
-        <v>0</v>
-      </c>
-      <c r="D141" t="n">
-        <v>33.22</v>
-      </c>
-      <c r="E141" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="n">
-        <v>55.12</v>
-      </c>
-      <c r="B142" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C142" t="n">
-        <v>0</v>
-      </c>
-      <c r="D142" t="n">
-        <v>33.4</v>
-      </c>
-      <c r="E142" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="n">
-        <v>55.36</v>
-      </c>
-      <c r="B143" t="n">
-        <v>791.6666666666803</v>
-      </c>
-      <c r="C143" t="n">
-        <v>0</v>
-      </c>
-      <c r="D143" t="n">
-        <v>33.59</v>
-      </c>
-      <c r="E143" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="n">
-        <v>55.61</v>
-      </c>
-      <c r="B144" t="n">
-        <v>759.9999999999909</v>
-      </c>
-      <c r="C144" t="n">
-        <v>0</v>
-      </c>
-      <c r="D144" t="n">
-        <v>33.78</v>
-      </c>
-      <c r="E144" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="n">
-        <v>55.85</v>
-      </c>
-      <c r="B145" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C145" t="n">
-        <v>0</v>
-      </c>
-      <c r="D145" t="n">
-        <v>33.96</v>
-      </c>
-      <c r="E145" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="n">
-        <v>56.09</v>
-      </c>
-      <c r="B146" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C146" t="n">
-        <v>0</v>
-      </c>
-      <c r="D146" t="n">
-        <v>34.15</v>
-      </c>
-      <c r="E146" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="n">
-        <v>56.33</v>
-      </c>
-      <c r="B147" t="n">
-        <v>791.6666666667037</v>
-      </c>
-      <c r="C147" t="n">
-        <v>0</v>
-      </c>
-      <c r="D147" t="n">
-        <v>34.34</v>
-      </c>
-      <c r="E147" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="n">
-        <v>56.58</v>
-      </c>
-      <c r="B148" t="n">
-        <v>719.9999999999989</v>
-      </c>
-      <c r="C148" t="n">
-        <v>0</v>
-      </c>
-      <c r="D148" t="n">
-        <v>34.52</v>
-      </c>
-      <c r="E148" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="n">
-        <v>56.82</v>
-      </c>
-      <c r="B149" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C149" t="n">
-        <v>0</v>
-      </c>
-      <c r="D149" t="n">
-        <v>34.71</v>
-      </c>
-      <c r="E149" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="n">
-        <v>57.06</v>
-      </c>
-      <c r="B150" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C150" t="n">
-        <v>0</v>
-      </c>
-      <c r="D150" t="n">
-        <v>34.9</v>
-      </c>
-      <c r="E150" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>57.3</v>
-      </c>
-      <c r="B151" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C151" t="n">
-        <v>0</v>
-      </c>
-      <c r="D151" t="n">
-        <v>35.08</v>
-      </c>
-      <c r="E151" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="n">
-        <v>57.54</v>
-      </c>
-      <c r="B152" t="n">
-        <v>791.6666666666803</v>
-      </c>
-      <c r="C152" t="n">
-        <v>0</v>
-      </c>
-      <c r="D152" t="n">
-        <v>35.27</v>
-      </c>
-      <c r="E152" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="n">
-        <v>57.78</v>
-      </c>
-      <c r="B153" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C153" t="n">
-        <v>0</v>
-      </c>
-      <c r="D153" t="n">
-        <v>35.46</v>
-      </c>
-      <c r="E153" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="n">
-        <v>58.02</v>
-      </c>
-      <c r="B154" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C154" t="n">
-        <v>0</v>
-      </c>
-      <c r="D154" t="n">
-        <v>35.64</v>
-      </c>
-      <c r="E154" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="n">
-        <v>58.26</v>
-      </c>
-      <c r="B155" t="n">
-        <v>791.666666666674</v>
-      </c>
-      <c r="C155" t="n">
-        <v>0</v>
-      </c>
-      <c r="D155" t="n">
-        <v>35.83</v>
-      </c>
-      <c r="E155" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="n">
-        <v>58.5</v>
-      </c>
-      <c r="B156" t="n">
-        <v>791.6666666666803</v>
-      </c>
-      <c r="C156" t="n">
-        <v>0</v>
-      </c>
-      <c r="D156" t="n">
-        <v>36.02</v>
-      </c>
-      <c r="E156" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="n">
-        <v>58.74</v>
-      </c>
-      <c r="B157" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C157" t="n">
-        <v>0</v>
-      </c>
-      <c r="D157" t="n">
-        <v>36.21</v>
-      </c>
-      <c r="E157" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="n">
-        <v>58.98</v>
-      </c>
-      <c r="B158" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C158" t="n">
-        <v>0</v>
-      </c>
-      <c r="D158" t="n">
-        <v>36.39</v>
-      </c>
-      <c r="E158" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="n">
-        <v>59.22</v>
-      </c>
-      <c r="B159" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C159" t="n">
-        <v>0</v>
-      </c>
-      <c r="D159" t="n">
-        <v>36.58</v>
-      </c>
-      <c r="E159" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="n">
-        <v>59.46</v>
-      </c>
-      <c r="B160" t="n">
-        <v>791.6666666666803</v>
-      </c>
-      <c r="C160" t="n">
-        <v>0</v>
-      </c>
-      <c r="D160" t="n">
-        <v>36.77</v>
-      </c>
-      <c r="E160" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="n">
-        <v>59.7</v>
-      </c>
-      <c r="B161" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C161" t="n">
-        <v>0</v>
-      </c>
-      <c r="D161" t="n">
-        <v>36.95</v>
-      </c>
-      <c r="E161" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="n">
-        <v>59.94</v>
-      </c>
-      <c r="B162" t="n">
-        <v>791.666666666674</v>
-      </c>
-      <c r="C162" t="n">
-        <v>0</v>
-      </c>
-      <c r="D162" t="n">
-        <v>37.14</v>
-      </c>
-      <c r="E162" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="n">
-        <v>60.18</v>
-      </c>
-      <c r="B163" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C163" t="n">
-        <v>0</v>
-      </c>
-      <c r="D163" t="n">
-        <v>37.33</v>
-      </c>
-      <c r="E163" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="n">
-        <v>60.42</v>
-      </c>
-      <c r="B164" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C164" t="n">
-        <v>0</v>
-      </c>
-      <c r="D164" t="n">
-        <v>37.51</v>
-      </c>
-      <c r="E164" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="n">
-        <v>60.65</v>
-      </c>
-      <c r="B165" t="n">
-        <v>826.0869565217713</v>
-      </c>
-      <c r="C165" t="n">
-        <v>0</v>
-      </c>
-      <c r="D165" t="n">
-        <v>37.7</v>
-      </c>
-      <c r="E165" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="n">
-        <v>60.89</v>
-      </c>
-      <c r="B166" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C166" t="n">
-        <v>0</v>
-      </c>
-      <c r="D166" t="n">
-        <v>37.89</v>
-      </c>
-      <c r="E166" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="n">
-        <v>61.13</v>
-      </c>
-      <c r="B167" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C167" t="n">
-        <v>0</v>
-      </c>
-      <c r="D167" t="n">
-        <v>38.07</v>
-      </c>
-      <c r="E167" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="n">
-        <v>61.37</v>
-      </c>
-      <c r="B168" t="n">
-        <v>791.666666666674</v>
-      </c>
-      <c r="C168" t="n">
-        <v>0</v>
-      </c>
-      <c r="D168" t="n">
-        <v>38.26</v>
-      </c>
-      <c r="E168" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="n">
-        <v>61.6</v>
-      </c>
-      <c r="B169" t="n">
-        <v>826.0869565217458</v>
-      </c>
-      <c r="C169" t="n">
-        <v>0</v>
-      </c>
-      <c r="D169" t="n">
-        <v>38.45</v>
-      </c>
-      <c r="E169" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="n">
-        <v>61.84</v>
-      </c>
-      <c r="B170" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C170" t="n">
-        <v>0</v>
-      </c>
-      <c r="D170" t="n">
-        <v>38.63</v>
-      </c>
-      <c r="E170" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="n">
-        <v>62.08</v>
-      </c>
-      <c r="B171" t="n">
-        <v>791.666666666674</v>
-      </c>
-      <c r="C171" t="n">
-        <v>0</v>
-      </c>
-      <c r="D171" t="n">
-        <v>38.82</v>
-      </c>
-      <c r="E171" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="n">
-        <v>62.31</v>
-      </c>
-      <c r="B172" t="n">
-        <v>826.0869565217149</v>
-      </c>
-      <c r="C172" t="n">
-        <v>0</v>
-      </c>
-      <c r="D172" t="n">
-        <v>39.01</v>
-      </c>
-      <c r="E172" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="n">
-        <v>62.55</v>
-      </c>
-      <c r="B173" t="n">
-        <v>791.6666666667037</v>
-      </c>
-      <c r="C173" t="n">
-        <v>0</v>
-      </c>
-      <c r="D173" t="n">
-        <v>39.2</v>
-      </c>
-      <c r="E173" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="n">
-        <v>62.78</v>
-      </c>
-      <c r="B174" t="n">
-        <v>782.6086956521592</v>
-      </c>
-      <c r="C174" t="n">
-        <v>0</v>
-      </c>
-      <c r="D174" t="n">
-        <v>39.38</v>
-      </c>
-      <c r="E174" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="n">
-        <v>63.02</v>
-      </c>
-      <c r="B175" t="n">
-        <v>791.6666666666506</v>
-      </c>
-      <c r="C175" t="n">
-        <v>0</v>
-      </c>
-      <c r="D175" t="n">
-        <v>39.57</v>
-      </c>
-      <c r="E175" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="n">
-        <v>63.25</v>
-      </c>
-      <c r="B176" t="n">
-        <v>826.0869565217405</v>
-      </c>
-      <c r="C176" t="n">
-        <v>0</v>
-      </c>
-      <c r="D176" t="n">
-        <v>39.76</v>
-      </c>
-      <c r="E176" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="n">
-        <v>63.49</v>
-      </c>
-      <c r="B177" t="n">
-        <v>749.9999999999926</v>
-      </c>
-      <c r="C177" t="n">
-        <v>0</v>
-      </c>
-      <c r="D177" t="n">
-        <v>39.94</v>
-      </c>
-      <c r="E177" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="n">
-        <v>63.72</v>
-      </c>
-      <c r="B178" t="n">
-        <v>826.0869565217713</v>
-      </c>
-      <c r="C178" t="n">
-        <v>0</v>
-      </c>
-      <c r="D178" t="n">
-        <v>40.13</v>
-      </c>
-      <c r="E178" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="n">
-        <v>63.97</v>
-      </c>
-      <c r="B179" t="n">
-        <v>759.9999999999909</v>
-      </c>
-      <c r="C179" t="n">
-        <v>0</v>
-      </c>
-      <c r="D179" t="n">
-        <v>40.32</v>
-      </c>
-      <c r="E179" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="n">
-        <v>64.19</v>
-      </c>
-      <c r="B180" t="n">
-        <v>818.1818181818211</v>
-      </c>
-      <c r="C180" t="n">
-        <v>0</v>
-      </c>
-      <c r="D180" t="n">
-        <v>40.5</v>
-      </c>
-      <c r="E180" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="n">
-        <v>64.43000000000001</v>
-      </c>
-      <c r="B181" t="n">
-        <v>791.6666666666272</v>
-      </c>
-      <c r="C181" t="n">
-        <v>0</v>
-      </c>
-      <c r="D181" t="n">
-        <v>40.69</v>
-      </c>
-      <c r="E181" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="n">
-        <v>64.66</v>
-      </c>
-      <c r="B182" t="n">
-        <v>826.0869565217969</v>
-      </c>
-      <c r="C182" t="n">
-        <v>0</v>
-      </c>
-      <c r="D182" t="n">
-        <v>40.88</v>
-      </c>
-      <c r="E182" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="n">
-        <v>64.90000000000001</v>
-      </c>
-      <c r="B183" t="n">
-        <v>749.9999999999703</v>
-      </c>
-      <c r="C183" t="n">
-        <v>0</v>
-      </c>
-      <c r="D183" t="n">
-        <v>41.06</v>
-      </c>
-      <c r="E183" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="n">
-        <v>65.13</v>
-      </c>
-      <c r="B184" t="n">
-        <v>826.086956521766</v>
-      </c>
-      <c r="C184" t="n">
-        <v>0</v>
-      </c>
-      <c r="D184" t="n">
-        <v>41.25</v>
-      </c>
-      <c r="E184" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="n">
-        <v>65.36</v>
-      </c>
-      <c r="B185" t="n">
-        <v>826.0869565217149</v>
-      </c>
-      <c r="C185" t="n">
-        <v>0</v>
-      </c>
-      <c r="D185" t="n">
-        <v>41.44</v>
-      </c>
-      <c r="E185" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="n">
-        <v>65.59999999999999</v>
-      </c>
-      <c r="B186" t="n">
-        <v>750.0000000000148</v>
-      </c>
-      <c r="C186" t="n">
-        <v>0</v>
-      </c>
-      <c r="D186" t="n">
-        <v>41.62</v>
-      </c>
-      <c r="E186" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="n">
-        <v>65.83</v>
-      </c>
-      <c r="B187" t="n">
-        <v>826.0869565217458</v>
-      </c>
-      <c r="C187" t="n">
-        <v>0</v>
-      </c>
-      <c r="D187" t="n">
-        <v>41.81</v>
-      </c>
-      <c r="E187" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="n">
-        <v>66.06</v>
-      </c>
-      <c r="B188" t="n">
-        <v>826.0869565217149</v>
-      </c>
-      <c r="C188" t="n">
-        <v>0</v>
-      </c>
-      <c r="D188" t="n">
-        <v>42</v>
-      </c>
-      <c r="E188" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="n">
-        <v>66.31844919786097</v>
-      </c>
-      <c r="C189" t="n">
-        <v>0</v>
-      </c>
-      <c r="D189" t="n">
-        <v>42.18181818181818</v>
-      </c>
-      <c r="E189" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>